<commit_message>
Mejores valores que pueden servir para seguir, pero ahora se intentara con 3 capas profundas
</commit_message>
<xml_diff>
--- a/Tesis/Resultados/Fundamentacion Ajuste Modelo/Resultados_Rango/Resultados_Rango_stateless.xlsx
+++ b/Tesis/Resultados/Fundamentacion Ajuste Modelo/Resultados_Rango/Resultados_Rango_stateless.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{05D5EA54-F4A6-49D8-BF2B-70CAEE15EBC4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CABA64-E8D5-4DC3-A068-6D3B9BDBA699}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10800" windowWidth="22260" windowHeight="12645" tabRatio="670" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="670" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AC_ACOSTADO" sheetId="1" r:id="rId1"/>
@@ -16,17 +16,23 @@
     <sheet name="CS_SENTADO" sheetId="6" r:id="rId6"/>
     <sheet name="Analisis Rango" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6130" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6135" uniqueCount="741">
   <si>
     <t>batch_size</t>
   </si>
@@ -2246,6 +2252,9 @@
   </si>
   <si>
     <t>DES EST</t>
+  </si>
+  <si>
+    <t>Dropout</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2418,11 +2427,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2457,11 +2479,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -5202,7 +5340,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>419923</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>57054</xdr:rowOff>
+      <xdr:rowOff>34642</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5410,23 +5548,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>9141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E459B00D-C9F7-463F-8776-DFDD02C56823}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905500" y="26445882"/>
+          <a:ext cx="6813176" cy="5119024"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3B22C7E-9288-4550-AFF0-A67CCFD28919}" name="Tabla1" displayName="Tabla1" ref="A3:E14" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3B22C7E-9288-4550-AFF0-A67CCFD28919}" name="Tabla1" displayName="Tabla1" ref="A3:E14" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A3:E14" xr:uid="{E9E8B13B-9F03-4CE0-8968-3E790BD8B0B0}"/>
-  <sortState ref="A4:E14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E14">
     <sortCondition descending="1" ref="D3:D14"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{65333096-056B-480D-A905-B2C6F5F7A790}" name="Epochs" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{65333096-056B-480D-A905-B2C6F5F7A790}" name="Epochs" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{BACD5F35-16FB-4CC4-8DEB-2A7806FFA257}" name="M Z"/>
-    <tableColumn id="3" xr3:uid="{2BD3396E-1271-4869-9DC7-35098F8AA8ED}" name="DE Z" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2BD3396E-1271-4869-9DC7-35098F8AA8ED}" name="DE Z" dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{4FF15169-50DE-4FE7-855A-24E9A9746590}" name="M R">
       <calculatedColumnFormula>TANH(B4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{996928D8-107E-47F3-BBF4-0508271AB29E}" name="DE R" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{996928D8-107E-47F3-BBF4-0508271AB29E}" name="DE R" dataDxfId="25">
       <calculatedColumnFormula>TANH(C4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5435,14 +5617,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3600967D-FC25-4075-B707-6B4FF77CA460}" name="Tabla2" displayName="Tabla2" ref="A17:E23" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3600967D-FC25-4075-B707-6B4FF77CA460}" name="Tabla2" displayName="Tabla2" ref="A17:E23" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A17:E23" xr:uid="{FDDF51AC-0166-4205-9D33-01755C009E6F}"/>
-  <sortState ref="A18:E23">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:E23">
     <sortCondition descending="1" ref="D17:D23"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A3EA63B-CE3F-4997-9688-0F895C348DC9}" name="Activation" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{299D640B-94B5-4C20-B5BB-779AC7840B45}" name="M Z" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{4A3EA63B-CE3F-4997-9688-0F895C348DC9}" name="Activation" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{299D640B-94B5-4C20-B5BB-779AC7840B45}" name="M Z" dataDxfId="20"/>
     <tableColumn id="3" xr3:uid="{9FC7F231-D16E-42FE-83A0-4D5F87DA14FB}" name="DE Z"/>
     <tableColumn id="4" xr3:uid="{8BEFF46E-41A8-4A10-B56B-938B2A32A07C}" name="M R">
       <calculatedColumnFormula>TANH(B18)</calculatedColumnFormula>
@@ -5456,14 +5638,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{26A41F2A-603F-4308-BC1C-14369BE944E2}" name="Tabla3" displayName="Tabla3" ref="A26:E33" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{26A41F2A-603F-4308-BC1C-14369BE944E2}" name="Tabla3" displayName="Tabla3" ref="A26:E33" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A26:E33" xr:uid="{56F3258C-C4C5-4FEC-B74D-3B6E8648102B}"/>
-  <sortState ref="A27:E33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:E33">
     <sortCondition descending="1" ref="D26:D33"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B2058491-46FD-4E5C-9874-1D2AB441B78E}" name="optimization" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{01987C03-B7FA-48C0-8695-4EB539A917BC}" name="M Z" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B2058491-46FD-4E5C-9874-1D2AB441B78E}" name="optimization" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{01987C03-B7FA-48C0-8695-4EB539A917BC}" name="M Z" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{748705B7-998C-4979-903A-A1CB0083FC03}" name="DE Z"/>
     <tableColumn id="4" xr3:uid="{693F89E8-42BC-4DBC-A046-385AE4C5788F}" name="M R">
       <calculatedColumnFormula>TANH(B27)</calculatedColumnFormula>
@@ -5477,14 +5659,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{292C6455-781B-4C7A-A626-84E9D0FBBED2}" name="Tabla4" displayName="Tabla4" ref="A36:E46" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{292C6455-781B-4C7A-A626-84E9D0FBBED2}" name="Tabla4" displayName="Tabla4" ref="A36:E46" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A36:E46" xr:uid="{E81D4E69-6587-4F89-A438-8E9111445684}"/>
-  <sortState ref="A37:E46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A37:E46">
     <sortCondition descending="1" ref="D36:D46"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{182CCF65-F7C8-45C3-A957-F30DDB097812}" name="Neurons" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1736AFF7-0AAD-4DF7-8D73-0475A5F02B8E}" name="M Z" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{182CCF65-F7C8-45C3-A957-F30DDB097812}" name="Neurons" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{1736AFF7-0AAD-4DF7-8D73-0475A5F02B8E}" name="M Z" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{ED183424-1549-4C23-93EC-D65FAFC83CF7}" name="DE Z"/>
     <tableColumn id="4" xr3:uid="{0B60D210-D683-489D-AE4D-8FFAAE817132}" name="M R">
       <calculatedColumnFormula>TANH(B37)</calculatedColumnFormula>
@@ -5498,20 +5680,43 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B0C3A9CC-EBD7-4BF8-BE8F-5E17C4788AF6}" name="Tabla5" displayName="Tabla5" ref="A49:E53" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B0C3A9CC-EBD7-4BF8-BE8F-5E17C4788AF6}" name="Tabla5" displayName="Tabla5" ref="A49:E53" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A49:E53" xr:uid="{543B011E-7B70-49FC-A979-D2DDAD0738BD}"/>
-  <sortState ref="A50:E53">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A50:E53">
     <sortCondition descending="1" ref="D49:D53"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6C5904B2-BA4D-47D0-AA51-61659506CFA4}" name="hidden_layers" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{8749F0FE-84E8-4678-835E-AEF3C3681830}" name="M Z" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6C5904B2-BA4D-47D0-AA51-61659506CFA4}" name="hidden_layers" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8749F0FE-84E8-4678-835E-AEF3C3681830}" name="M Z" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{408D9A1F-AC4F-4F19-85A2-9EE02F768386}" name="DE Z"/>
     <tableColumn id="4" xr3:uid="{D26A8C91-F6CE-4306-B679-21F6C205EB41}" name="M R">
       <calculatedColumnFormula>TANH(B50)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{1D3FB3E6-3B00-4269-881A-BA9BE8DE6DC5}" name="DE R">
       <calculatedColumnFormula>TANH(C50)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E5A28D12-C99F-4F62-9626-742CAEB7E36E}" name="Tabla47" displayName="Tabla47" ref="A56:E67" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
+  <autoFilter ref="A56:E67" xr:uid="{289C6B8B-B70E-4F93-A582-9E5818B4F472}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A57:E67">
+    <sortCondition descending="1" ref="D56:D67"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FBF4EE49-1BCB-4794-BE1B-4F7A8E864B0E}" name="Dropout" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B5433562-8336-4B26-9871-6DE7CCB08209}" name="M Z" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{64206578-437B-4BB0-8DF6-BCB86F62B455}" name="DE Z" dataDxfId="0">
+      <calculatedColumnFormula>STDEVA(AC_ACOSTADO!J27,AC_ACOSTADO!U27,DM_PIE!J27,DM_PIE!U23,PC_SENTADO!J23,PC_SENTADO!U23,AV_ACOSTADO!J20,AV_ACOSTADO!U20,CC_PIE!J20,CC_PIE!U20,CS_SENTADO!J20,CS_SENTADO!U20)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{9508A7FF-068A-4334-8587-6D79CFBABB17}" name="M R">
+      <calculatedColumnFormula>TANH(B57)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F40C6A32-7A34-49BB-9B68-A331929A0FEB}" name="DE R">
+      <calculatedColumnFormula>TANH(C57)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5784,7 +5989,7 @@
   <dimension ref="B4:V74"/>
   <sheetViews>
     <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9276,7 +9481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1211BBCB-56DF-469C-8EC6-0285F1D042C8}">
   <dimension ref="B5:V81"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
@@ -13116,7 +13321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5A3430-3DF6-4B02-9F42-21571F075A3E}">
   <dimension ref="B4:V84"/>
   <sheetViews>
-    <sheetView topLeftCell="C41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V82" sqref="V82"/>
     </sheetView>
   </sheetViews>
@@ -17189,7 +17394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9EA154-AEAD-4D93-A5ED-99077536C013}">
   <dimension ref="B4:V73"/>
   <sheetViews>
-    <sheetView topLeftCell="D38" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="V71" sqref="V71"/>
     </sheetView>
   </sheetViews>
@@ -20622,7 +20827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9235D6-A631-4E39-9897-7FD20878CBF8}">
   <dimension ref="B4:V83"/>
   <sheetViews>
-    <sheetView topLeftCell="C39" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="V81" sqref="V81"/>
     </sheetView>
   </sheetViews>
@@ -24636,7 +24841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E8F959-5E75-4E54-9A00-F421BEB1FD9E}">
   <dimension ref="B4:V73"/>
   <sheetViews>
-    <sheetView topLeftCell="C39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V71" sqref="V71"/>
     </sheetView>
   </sheetViews>
@@ -28068,10 +28273,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4240923-B78A-47DB-A92D-14820FEEC601}">
-  <dimension ref="A3:E53"/>
+  <dimension ref="A3:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="S148" sqref="S148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28965,16 +29170,265 @@
         <v>0.44522014666602983</v>
       </c>
     </row>
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
+        <v>740</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>735</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="B57" s="20">
+        <f>AVERAGE(AC_ACOSTADO!J30,AC_ACOSTADO!U20,DM_PIE!J21,DM_PIE!U21,PC_SENTADO!J20,PC_SENTADO!U20,AV_ACOSTADO!J20,AV_ACOSTADO!U20,CC_PIE!J20,CC_PIE!U20,CS_SENTADO!J20,CS_SENTADO!U21)</f>
+        <v>0.59808973106892893</v>
+      </c>
+      <c r="C57" s="20">
+        <f>STDEVA(AC_ACOSTADO!J30,AC_ACOSTADO!U20,DM_PIE!J21,DM_PIE!U21,PC_SENTADO!J20,PC_SENTADO!U20,AV_ACOSTADO!J20,AV_ACOSTADO!U20,CC_PIE!J20,CC_PIE!U20,CS_SENTADO!J20,CS_SENTADO!U21)</f>
+        <v>0.19872253889317226</v>
+      </c>
+      <c r="D57">
+        <f>TANH(B57)</f>
+        <v>0.53568886780756009</v>
+      </c>
+      <c r="E57">
+        <f>TANH(C57)</f>
+        <v>0.19614731623210999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="23">
+        <v>1</v>
+      </c>
+      <c r="B58" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J27,AC_ACOSTADO!U27,DM_PIE!J27,DM_PIE!U23,PC_SENTADO!J23,PC_SENTADO!U23,AV_ACOSTADO!J20,AV_ACOSTADO!U20,CC_PIE!J20,CC_PIE!U20,CS_SENTADO!J20,CS_SENTADO!U20)</f>
+        <v>0.57078730792385313</v>
+      </c>
+      <c r="C58" s="9">
+        <f>STDEVA(AC_ACOSTADO!J27,AC_ACOSTADO!U27,DM_PIE!J27,DM_PIE!U23,PC_SENTADO!J23,PC_SENTADO!U23,AV_ACOSTADO!J20,AV_ACOSTADO!U20,CC_PIE!J20,CC_PIE!U20,CS_SENTADO!J20,CS_SENTADO!U20)</f>
+        <v>0.19486635619976767</v>
+      </c>
+      <c r="D58">
+        <f>TANH(B58)</f>
+        <v>0.51593724610931757</v>
+      </c>
+      <c r="E58">
+        <f>TANH(C58)</f>
+        <v>0.19243670718580286</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="B59" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J29,AC_ACOSTADO!U21,DM_PIE!J22,DM_PIE!U22,PC_SENTADO!J21,PC_SENTADO!U21,AV_ACOSTADO!J22,AV_ACOSTADO!U21,CC_PIE!J22,CC_PIE!U23,CS_SENTADO!J21,CS_SENTADO!U27)</f>
+        <v>0.56888715088685016</v>
+      </c>
+      <c r="C59" s="9">
+        <f>STDEVA(AC_ACOSTADO!J29,AC_ACOSTADO!U21,DM_PIE!J22,DM_PIE!U22,PC_SENTADO!J21,PC_SENTADO!U21,AV_ACOSTADO!J22,AV_ACOSTADO!U21,CC_PIE!J22,CC_PIE!U23,CS_SENTADO!J21,CS_SENTADO!U27)</f>
+        <v>0.1910849035419788</v>
+      </c>
+      <c r="D59">
+        <f>TANH(B59)</f>
+        <v>0.51454152760454475</v>
+      </c>
+      <c r="E59">
+        <f>TANH(C59)</f>
+        <v>0.18879265448020346</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="B60" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J26,AC_ACOSTADO!U23,DM_PIE!J23,DM_PIE!U25,PC_SENTADO!J25,PC_SENTADO!U28,AV_ACOSTADO!J21,AV_ACOSTADO!U25,CC_PIE!J25,CC_PIE!U24,CS_SENTADO!J29,CS_SENTADO!U25)</f>
+        <v>0.55147655576355481</v>
+      </c>
+      <c r="C60" s="9">
+        <f>STDEVA(AC_ACOSTADO!J26,AC_ACOSTADO!U23,DM_PIE!J23,DM_PIE!U25,PC_SENTADO!J25,PC_SENTADO!U28,AV_ACOSTADO!J21,AV_ACOSTADO!U25,CC_PIE!J25,CC_PIE!U24,CS_SENTADO!J29,CS_SENTADO!U25)</f>
+        <v>0.1896384401281716</v>
+      </c>
+      <c r="D60">
+        <f>TANH(B60)</f>
+        <v>0.50162604142941747</v>
+      </c>
+      <c r="E60">
+        <f>TANH(C60)</f>
+        <v>0.18739736682491384</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="23">
+        <v>0</v>
+      </c>
+      <c r="B61" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J28,AC_ACOSTADO!U30,DM_PIE!J26,DM_PIE!U24,PC_SENTADO!J22,PC_SENTADO!U24,AV_ACOSTADO!J27,AV_ACOSTADO!U23,CC_PIE!J29,CC_PIE!U21,CS_SENTADO!J28,CS_SENTADO!U23)</f>
+        <v>0.55120587864835402</v>
+      </c>
+      <c r="C61" s="9">
+        <f>STDEVA(AC_ACOSTADO!J28,AC_ACOSTADO!U30,DM_PIE!J26,DM_PIE!U24,PC_SENTADO!J22,PC_SENTADO!U24,AV_ACOSTADO!J27,AV_ACOSTADO!U23,CC_PIE!J29,CC_PIE!U21,CS_SENTADO!J28,CS_SENTADO!U23)</f>
+        <v>0.18857588834152025</v>
+      </c>
+      <c r="D61">
+        <f>TANH(B61)</f>
+        <v>0.50142344693782659</v>
+      </c>
+      <c r="E61">
+        <f>TANH(C61)</f>
+        <v>0.18637192569148844</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="B62" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J21,AC_ACOSTADO!U26,DM_PIE!J31,DM_PIE!U28,PC_SENTADO!J29,PC_SENTADO!U27,AV_ACOSTADO!J24,AV_ACOSTADO!U22,CC_PIE!J27,CC_PIE!U27,CS_SENTADO!J24,CS_SENTADO!U20)</f>
+        <v>0.54553632713720857</v>
+      </c>
+      <c r="C62" s="9">
+        <f>STDEVA(AC_ACOSTADO!J21,AC_ACOSTADO!U26,DM_PIE!J31,DM_PIE!U28,PC_SENTADO!J29,PC_SENTADO!U27,AV_ACOSTADO!J24,AV_ACOSTADO!U22,CC_PIE!J27,CC_PIE!U27,CS_SENTADO!J24,CS_SENTADO!U20)</f>
+        <v>0.19382339958087277</v>
+      </c>
+      <c r="D62">
+        <f>TANH(B62)</f>
+        <v>0.49716731116174423</v>
+      </c>
+      <c r="E62">
+        <f>TANH(C62)</f>
+        <v>0.19143217196866683</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="B63" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J20,AC_ACOSTADO!U24,DM_PIE!J30,DM_PIE!U30,PC_SENTADO!J30,PC_SENTADO!U29,AV_ACOSTADO!J29,AV_ACOSTADO!U28,CC_PIE!J23,CC_PIE!U28,CS_SENTADO!J23,CS_SENTADO!U29)</f>
+        <v>0.54050342472458779</v>
+      </c>
+      <c r="C63" s="9">
+        <f>STDEVA(AC_ACOSTADO!J20,AC_ACOSTADO!U24,DM_PIE!J30,DM_PIE!U30,PC_SENTADO!J30,PC_SENTADO!U29,AV_ACOSTADO!J29,AV_ACOSTADO!U28,CC_PIE!J23,CC_PIE!U28,CS_SENTADO!J23,CS_SENTADO!U29)</f>
+        <v>0.19058634482611142</v>
+      </c>
+      <c r="D63">
+        <f>TANH(B63)</f>
+        <v>0.49336894591251595</v>
+      </c>
+      <c r="E63">
+        <f>TANH(C63)</f>
+        <v>0.18831182050803405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="B64" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J22,AC_ACOSTADO!U28,DM_PIE!J28,DM_PIE!U29,PC_SENTADO!J28,PC_SENTADO!U30,AV_ACOSTADO!J26,AV_ACOSTADO!U29,CC_PIE!J24,CC_PIE!U29,CS_SENTADO!J26,CS_SENTADO!U24)</f>
+        <v>0.53586945114048623</v>
+      </c>
+      <c r="C64" s="9">
+        <f>STDEVA(AC_ACOSTADO!J22,AC_ACOSTADO!U28,DM_PIE!J28,DM_PIE!U29,PC_SENTADO!J28,PC_SENTADO!U30,AV_ACOSTADO!J26,AV_ACOSTADO!U29,CC_PIE!J24,CC_PIE!U29,CS_SENTADO!J26,CS_SENTADO!U24)</f>
+        <v>0.18972761190606766</v>
+      </c>
+      <c r="D64">
+        <f>TANH(B64)</f>
+        <v>0.48985493256432766</v>
+      </c>
+      <c r="E64">
+        <f>TANH(C64)</f>
+        <v>0.18748340565056273</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="B65" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J23,AC_ACOSTADO!U25,DM_PIE!I25,DM_PIE!T31,PC_SENTADO!J26,PC_SENTADO!U22,AV_ACOSTADO!J28,AV_ACOSTADO!U27,CC_PIE!J21,CC_PIE!U22,CS_SENTADO!J22,CS_SENTADO!U26)</f>
+        <v>0.52523929158044458</v>
+      </c>
+      <c r="C65" s="9">
+        <f>STDEVA(AC_ACOSTADO!J23,AC_ACOSTADO!U25,DM_PIE!I25,DM_PIE!T31,PC_SENTADO!J26,PC_SENTADO!U22,AV_ACOSTADO!J28,AV_ACOSTADO!U27,CC_PIE!J21,CC_PIE!U22,CS_SENTADO!J22,CS_SENTADO!U26)</f>
+        <v>0.25459970423269901</v>
+      </c>
+      <c r="D65">
+        <f>TANH(B65)</f>
+        <v>0.48173357938957306</v>
+      </c>
+      <c r="E65">
+        <f>TANH(C65)</f>
+        <v>0.24923755675876738</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="B66" s="9">
+        <f>AVERAGE(AC_ACOSTADO!J25,AC_ACOSTADO!U22,DM_PIE!J24,DM_PIE!U27,PC_SENTADO!J27,PC_SENTADO!U26,AV_ACOSTADO!J23,AV_ACOSTADO!U24,CC_PIE!J28,CC_PIE!U25,CS_SENTADO!J27,CS_SENTADO!U28,)</f>
+        <v>0.50999324821567904</v>
+      </c>
+      <c r="C66" s="9">
+        <f>STDEVA(AC_ACOSTADO!J25,AC_ACOSTADO!U22,DM_PIE!J24,DM_PIE!U27,PC_SENTADO!J27,PC_SENTADO!U26,AV_ACOSTADO!J23,AV_ACOSTADO!U24,CC_PIE!J28,CC_PIE!U25,CS_SENTADO!J27,CS_SENTADO!U28,)</f>
+        <v>0.23880324913975146</v>
+      </c>
+      <c r="D66">
+        <f>TANH(B66)</f>
+        <v>0.46993993825339686</v>
+      </c>
+      <c r="E66">
+        <f>TANH(C66)</f>
+        <v>0.23436505025942772</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="B67" s="21">
+        <f>AVERAGE(AC_ACOSTADO!J24,AC_ACOSTADO!U29,DM_PIE!J29,DM_PIE!U26,PC_SENTADO!J24,PC_SENTADO!U25,AV_ACOSTADO!J25,AV_ACOSTADO!U26,CC_PIE!J26,CC_PIE!U26,CS_SENTADO!J25,CS_SENTADO!U22,)</f>
+        <v>0.50173919625758345</v>
+      </c>
+      <c r="C67" s="21">
+        <f>STDEVA(AC_ACOSTADO!J24,AC_ACOSTADO!U29,DM_PIE!J29,DM_PIE!U26,PC_SENTADO!J24,PC_SENTADO!U25,AV_ACOSTADO!J25,AV_ACOSTADO!U26,CC_PIE!J26,CC_PIE!U26,CS_SENTADO!J25,CS_SENTADO!U22,)</f>
+        <v>0.23633332743668109</v>
+      </c>
+      <c r="D67">
+        <f>TANH(B67)</f>
+        <v>0.46348384441252954</v>
+      </c>
+      <c r="E67">
+        <f>TANH(C67)</f>
+        <v>0.23202944664258288</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>